<commit_message>
Updated Tracking sheet to reflect revised resource list and proposal assignments
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@1306 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/governance/FMG/2013-05 QA Assignments.xlsx
+++ b/documents/governance/FMG/2013-05 QA Assignments.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="13290" activeTab="1"/>
+    <workbookView xWindow="18315" yWindow="90" windowWidth="9960" windowHeight="13290" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Review plans" sheetId="1" r:id="rId1"/>
     <sheet name="Participants" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Participants!$A$1:$D$23</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
   <si>
     <t>Topic</t>
   </si>
@@ -195,6 +198,30 @@
   </si>
   <si>
     <t>Descriptions</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Andy</t>
+  </si>
+  <si>
+    <t>Preferred topic</t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>regrets</t>
+  </si>
+  <si>
+    <t>will give more</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -694,10 +721,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,240 +732,317 @@
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="D19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>59</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D23"/>
   <sortState ref="A1:C16">
     <sortCondition ref="A1:A16"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
-    <hyperlink ref="C8" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
-    <hyperlink ref="C10" r:id="rId5"/>
-    <hyperlink ref="C16" r:id="rId6"/>
-    <hyperlink ref="C11" r:id="rId7"/>
-    <hyperlink ref="C15" r:id="rId8"/>
-    <hyperlink ref="C12" r:id="rId9"/>
-    <hyperlink ref="C13" r:id="rId10"/>
-    <hyperlink ref="C14" r:id="rId11"/>
-    <hyperlink ref="C9" r:id="rId12"/>
-    <hyperlink ref="C2" r:id="rId13"/>
-    <hyperlink ref="C1" r:id="rId14"/>
-    <hyperlink ref="C7" r:id="rId15"/>
-    <hyperlink ref="C4" r:id="rId16"/>
-    <hyperlink ref="C17" r:id="rId17"/>
-    <hyperlink ref="C18" r:id="rId18"/>
-    <hyperlink ref="C19" r:id="rId19"/>
-    <hyperlink ref="C20" r:id="rId20"/>
-    <hyperlink ref="C21" r:id="rId21"/>
+    <hyperlink ref="C7" r:id="rId1"/>
+    <hyperlink ref="C6" r:id="rId2"/>
+    <hyperlink ref="C9" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="C11" r:id="rId5"/>
+    <hyperlink ref="C17" r:id="rId6"/>
+    <hyperlink ref="C12" r:id="rId7"/>
+    <hyperlink ref="C16" r:id="rId8"/>
+    <hyperlink ref="C13" r:id="rId9"/>
+    <hyperlink ref="C14" r:id="rId10"/>
+    <hyperlink ref="C15" r:id="rId11"/>
+    <hyperlink ref="C10" r:id="rId12"/>
+    <hyperlink ref="C3" r:id="rId13"/>
+    <hyperlink ref="C2" r:id="rId14"/>
+    <hyperlink ref="C8" r:id="rId15"/>
+    <hyperlink ref="C5" r:id="rId16"/>
+    <hyperlink ref="C18" r:id="rId17"/>
+    <hyperlink ref="C19" r:id="rId18"/>
+    <hyperlink ref="C20" r:id="rId19"/>
+    <hyperlink ref="C21" r:id="rId20"/>
+    <hyperlink ref="C22" r:id="rId21"/>
+    <hyperlink ref="C23" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>